<commit_message>
resized images, added protocol selection and run dialog
</commit_message>
<xml_diff>
--- a/trials.xlsx
+++ b/trials.xlsx
@@ -14,63 +14,177 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
-  <si>
-    <t>imgpath</t>
-  </si>
-  <si>
-    <t>images/B1_</t>
-  </si>
-  <si>
-    <t>images/B2_</t>
-  </si>
-  <si>
-    <t>images/B3_</t>
-  </si>
-  <si>
-    <t>images/B4_</t>
-  </si>
-  <si>
-    <t>images/B5_</t>
-  </si>
-  <si>
-    <t>images/B6_</t>
-  </si>
-  <si>
-    <t>images/B7_</t>
-  </si>
-  <si>
-    <t>images/B8_</t>
-  </si>
-  <si>
-    <t>images/B9_</t>
-  </si>
-  <si>
-    <t>images/B10_</t>
-  </si>
-  <si>
-    <t>images/B11_</t>
-  </si>
-  <si>
-    <t>images/B12_</t>
-  </si>
-  <si>
-    <t>images/B13_</t>
-  </si>
-  <si>
-    <t>images/B14_</t>
-  </si>
-  <si>
-    <t>jitter</t>
-  </si>
-  <si>
-    <t>dur_a</t>
-  </si>
-  <si>
-    <t>dur_b</t>
-  </si>
-  <si>
-    <t>dur_c</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+  <si>
+    <t>images/high/B11_</t>
+  </si>
+  <si>
+    <t>images/high/B7_</t>
+  </si>
+  <si>
+    <t>images/high/B5_</t>
+  </si>
+  <si>
+    <t>images/high/B13_</t>
+  </si>
+  <si>
+    <t>images/high/B9_</t>
+  </si>
+  <si>
+    <t>images/high/B14_</t>
+  </si>
+  <si>
+    <t>images/high/B3_</t>
+  </si>
+  <si>
+    <t>images/high/B4_</t>
+  </si>
+  <si>
+    <t>images/high/B6_</t>
+  </si>
+  <si>
+    <t>images/high/B2_</t>
+  </si>
+  <si>
+    <t>images/high/B1_</t>
+  </si>
+  <si>
+    <t>images/high/B10_</t>
+  </si>
+  <si>
+    <t>images/high/B12_</t>
+  </si>
+  <si>
+    <t>images/high/B8_</t>
+  </si>
+  <si>
+    <t>high_imgpath</t>
+  </si>
+  <si>
+    <t>high_dur_a</t>
+  </si>
+  <si>
+    <t>high_dur_b</t>
+  </si>
+  <si>
+    <t>high_dur_c</t>
+  </si>
+  <si>
+    <t>high_jitter</t>
+  </si>
+  <si>
+    <t>low_imgpath</t>
+  </si>
+  <si>
+    <t>low_dur_a</t>
+  </si>
+  <si>
+    <t>low_dur_b</t>
+  </si>
+  <si>
+    <t>low_dur_c</t>
+  </si>
+  <si>
+    <t>low_jitter</t>
+  </si>
+  <si>
+    <t>scramble_imgpath</t>
+  </si>
+  <si>
+    <t>scramble_dur_a</t>
+  </si>
+  <si>
+    <t>scramble_dur_b</t>
+  </si>
+  <si>
+    <t>scramble_dur_c</t>
+  </si>
+  <si>
+    <t>scramble_jitter</t>
+  </si>
+  <si>
+    <t>images/low/B11_</t>
+  </si>
+  <si>
+    <t>images/low/B7_</t>
+  </si>
+  <si>
+    <t>images/low/B5_</t>
+  </si>
+  <si>
+    <t>images/low/B13_</t>
+  </si>
+  <si>
+    <t>images/low/B9_</t>
+  </si>
+  <si>
+    <t>images/low/B14_</t>
+  </si>
+  <si>
+    <t>images/low/B3_</t>
+  </si>
+  <si>
+    <t>images/low/B4_</t>
+  </si>
+  <si>
+    <t>images/low/B6_</t>
+  </si>
+  <si>
+    <t>images/low/B2_</t>
+  </si>
+  <si>
+    <t>images/low/B1_</t>
+  </si>
+  <si>
+    <t>images/low/B10_</t>
+  </si>
+  <si>
+    <t>images/low/B12_</t>
+  </si>
+  <si>
+    <t>images/low/B8_</t>
+  </si>
+  <si>
+    <t>images/scramble/B11_</t>
+  </si>
+  <si>
+    <t>images/scramble/B7_</t>
+  </si>
+  <si>
+    <t>images/scramble/B5_</t>
+  </si>
+  <si>
+    <t>images/scramble/B13_</t>
+  </si>
+  <si>
+    <t>images/scramble/B9_</t>
+  </si>
+  <si>
+    <t>images/scramble/B14_</t>
+  </si>
+  <si>
+    <t>images/scramble/B3_</t>
+  </si>
+  <si>
+    <t>images/scramble/B4_</t>
+  </si>
+  <si>
+    <t>images/scramble/B6_</t>
+  </si>
+  <si>
+    <t>images/scramble/B2_</t>
+  </si>
+  <si>
+    <t>images/scramble/B1_</t>
+  </si>
+  <si>
+    <t>images/scramble/B10_</t>
+  </si>
+  <si>
+    <t>images/scramble/B12_</t>
+  </si>
+  <si>
+    <t>images/scramble/B8_</t>
   </si>
 </sst>
 </file>
@@ -412,41 +526,77 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.88671875" customWidth="1"/>
-    <col min="5" max="5" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="10.109375" customWidth="1"/>
+    <col min="11" max="11" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" t="s">
+        <v>27</v>
+      </c>
+      <c r="O1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
       <c r="B2">
         <v>1</v>
       </c>
@@ -459,10 +609,40 @@
       <c r="E2">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2">
+        <v>4</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <v>1.5</v>
+      </c>
+      <c r="J2">
+        <v>4</v>
+      </c>
+      <c r="K2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L2">
+        <v>3.5</v>
+      </c>
+      <c r="M2">
+        <v>1.5</v>
+      </c>
+      <c r="N2">
+        <v>2.5</v>
+      </c>
+      <c r="O2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -476,10 +656,40 @@
       <c r="E3">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+      <c r="H3">
+        <v>3.5</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>2</v>
+      </c>
+      <c r="K3" t="s">
+        <v>54</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>4</v>
+      </c>
+      <c r="N3">
+        <v>2.5</v>
+      </c>
+      <c r="O3">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>4</v>
@@ -493,10 +703,40 @@
       <c r="E4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>3</v>
+      </c>
+      <c r="I4">
+        <v>3.5</v>
+      </c>
+      <c r="J4">
+        <v>3.5</v>
+      </c>
+      <c r="K4" t="s">
+        <v>48</v>
+      </c>
+      <c r="L4">
+        <v>4</v>
+      </c>
+      <c r="M4">
+        <v>2</v>
+      </c>
+      <c r="N4">
+        <v>1.5</v>
+      </c>
+      <c r="O4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>1.5</v>
@@ -510,10 +750,40 @@
       <c r="E5">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5">
+        <v>1.5</v>
+      </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
+      <c r="I5">
+        <v>2</v>
+      </c>
+      <c r="J5">
+        <v>6</v>
+      </c>
+      <c r="K5" t="s">
+        <v>56</v>
+      </c>
+      <c r="L5">
+        <v>2</v>
+      </c>
+      <c r="M5">
+        <v>3</v>
+      </c>
+      <c r="N5">
+        <v>2.5</v>
+      </c>
+      <c r="O5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -527,10 +797,40 @@
       <c r="E6">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6">
+        <v>1.5</v>
+      </c>
+      <c r="H6">
+        <v>3.5</v>
+      </c>
+      <c r="I6">
+        <v>2.5</v>
+      </c>
+      <c r="J6">
+        <v>3</v>
+      </c>
+      <c r="K6" t="s">
+        <v>53</v>
+      </c>
+      <c r="L6">
+        <v>2.5</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>4</v>
+      </c>
+      <c r="O6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>2.5</v>
@@ -544,10 +844,40 @@
       <c r="E7">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7">
+        <v>2.5</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>4</v>
+      </c>
+      <c r="J7">
+        <v>5</v>
+      </c>
+      <c r="K7" t="s">
+        <v>46</v>
+      </c>
+      <c r="L7">
+        <v>1.5</v>
+      </c>
+      <c r="M7">
+        <v>4</v>
+      </c>
+      <c r="N7">
+        <v>2</v>
+      </c>
+      <c r="O7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>4</v>
@@ -561,10 +891,40 @@
       <c r="E8">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F8" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8">
+        <v>2.5</v>
+      </c>
+      <c r="H8">
+        <v>3</v>
+      </c>
+      <c r="I8">
+        <v>2</v>
+      </c>
+      <c r="J8">
+        <v>3</v>
+      </c>
+      <c r="K8" t="s">
+        <v>51</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <v>3</v>
+      </c>
+      <c r="N8">
+        <v>3.5</v>
+      </c>
+      <c r="O8">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>3.5</v>
@@ -578,10 +938,40 @@
       <c r="E9">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F9" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9">
+        <v>4</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>2.5</v>
+      </c>
+      <c r="J9">
+        <v>6</v>
+      </c>
+      <c r="K9" t="s">
+        <v>49</v>
+      </c>
+      <c r="L9">
+        <v>4</v>
+      </c>
+      <c r="M9">
+        <v>1</v>
+      </c>
+      <c r="N9">
+        <v>2.5</v>
+      </c>
+      <c r="O9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>2</v>
@@ -595,10 +985,40 @@
       <c r="E10">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F10" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10">
+        <v>3.5</v>
+      </c>
+      <c r="H10">
+        <v>1.5</v>
+      </c>
+      <c r="I10">
+        <v>2.5</v>
+      </c>
+      <c r="J10">
+        <v>2</v>
+      </c>
+      <c r="K10" t="s">
+        <v>44</v>
+      </c>
+      <c r="L10">
+        <v>4</v>
+      </c>
+      <c r="M10">
+        <v>2</v>
+      </c>
+      <c r="N10">
+        <v>1.5</v>
+      </c>
+      <c r="O10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>2.5</v>
@@ -612,10 +1032,40 @@
       <c r="E11">
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F11" t="s">
+        <v>37</v>
+      </c>
+      <c r="G11">
+        <v>4</v>
+      </c>
+      <c r="H11">
+        <v>2</v>
+      </c>
+      <c r="I11">
+        <v>1.5</v>
+      </c>
+      <c r="J11">
+        <v>5</v>
+      </c>
+      <c r="K11" t="s">
+        <v>47</v>
+      </c>
+      <c r="L11">
+        <v>2</v>
+      </c>
+      <c r="M11">
+        <v>2.5</v>
+      </c>
+      <c r="N11">
+        <v>3</v>
+      </c>
+      <c r="O11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>4</v>
@@ -629,10 +1079,40 @@
       <c r="E12">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F12" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12">
+        <v>2</v>
+      </c>
+      <c r="H12">
+        <v>3</v>
+      </c>
+      <c r="I12">
+        <v>2.5</v>
+      </c>
+      <c r="J12">
+        <v>7</v>
+      </c>
+      <c r="K12" t="s">
+        <v>55</v>
+      </c>
+      <c r="L12">
+        <v>1.5</v>
+      </c>
+      <c r="M12">
+        <v>3.5</v>
+      </c>
+      <c r="N12">
+        <v>2.5</v>
+      </c>
+      <c r="O12">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>3</v>
@@ -646,8 +1126,38 @@
       <c r="E13">
         <v>9</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G13">
+        <v>2</v>
+      </c>
+      <c r="H13">
+        <v>2.5</v>
+      </c>
+      <c r="I13">
+        <v>3</v>
+      </c>
+      <c r="J13">
+        <v>4.5</v>
+      </c>
+      <c r="K13" t="s">
+        <v>52</v>
+      </c>
+      <c r="L13">
+        <v>2.5</v>
+      </c>
+      <c r="M13">
+        <v>3</v>
+      </c>
+      <c r="N13">
+        <v>2</v>
+      </c>
+      <c r="O13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -663,10 +1173,40 @@
       <c r="E14">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F14" t="s">
+        <v>40</v>
+      </c>
+      <c r="G14">
+        <v>2.5</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>4</v>
+      </c>
+      <c r="J14">
+        <v>9</v>
+      </c>
+      <c r="K14" t="s">
+        <v>43</v>
+      </c>
+      <c r="L14">
+        <v>2.5</v>
+      </c>
+      <c r="M14">
+        <v>1</v>
+      </c>
+      <c r="N14">
+        <v>4</v>
+      </c>
+      <c r="O14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>2.5</v>
@@ -678,6 +1218,36 @@
         <v>4</v>
       </c>
       <c r="E15">
+        <v>3</v>
+      </c>
+      <c r="F15" t="s">
+        <v>36</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>4</v>
+      </c>
+      <c r="I15">
+        <v>2.5</v>
+      </c>
+      <c r="J15">
+        <v>3</v>
+      </c>
+      <c r="K15" t="s">
+        <v>45</v>
+      </c>
+      <c r="L15">
+        <v>3</v>
+      </c>
+      <c r="M15">
+        <v>3.5</v>
+      </c>
+      <c r="N15">
+        <v>1</v>
+      </c>
+      <c r="O15">
         <v>3</v>
       </c>
     </row>

</xml_diff>